<commit_message>
Updated data files, added new analysis outputs and visuals
</commit_message>
<xml_diff>
--- a/Station_Time_Metadata.xlsx
+++ b/Station_Time_Metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa-marieweidl/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa-marieweidl/PyCharmDesktop/ML Water/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688C5EF9-ADE1-7849-AA5F-D0DBBD4788BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23FA3C0-27AC-D345-86D0-D0A70991FE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="19360" windowHeight="11360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="4480" windowWidth="19360" windowHeight="11360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Station_ID</t>
   </si>
@@ -31,12 +31,6 @@
     <t>End_Date</t>
   </si>
   <si>
-    <t>Measurement_Count</t>
-  </si>
-  <si>
-    <t>Avg_Frequency_Days</t>
-  </si>
-  <si>
     <t>PG31000292</t>
   </si>
   <si>
@@ -65,6 +59,9 @@
   </si>
   <si>
     <t>PG32500392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement (N)_Total </t>
   </si>
 </sst>
 </file>
@@ -74,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +86,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,12 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -436,21 +440,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,15 +465,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>33330</v>
@@ -477,16 +478,13 @@
       <c r="C2" s="2">
         <v>45594</v>
       </c>
-      <c r="D2">
-        <v>84</v>
-      </c>
-      <c r="E2">
-        <v>147.75903614457829</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="3">
+        <v>93408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>33339</v>
@@ -494,16 +492,13 @@
       <c r="C3" s="2">
         <v>45594</v>
       </c>
-      <c r="D3">
-        <v>83</v>
-      </c>
-      <c r="E3">
-        <v>149.45121951219511</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="3">
+        <v>92296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>33330</v>
@@ -511,16 +506,13 @@
       <c r="C4" s="2">
         <v>45593</v>
       </c>
-      <c r="D4">
-        <v>82</v>
-      </c>
-      <c r="E4">
-        <v>151.39506172839509</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="3">
+        <v>91184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>34625</v>
@@ -528,16 +520,13 @@
       <c r="C5" s="2">
         <v>45593</v>
       </c>
-      <c r="D5">
-        <v>83</v>
-      </c>
-      <c r="E5">
-        <v>133.7560975609756</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="3">
+        <v>92296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>33330</v>
@@ -545,16 +534,13 @@
       <c r="C6" s="2">
         <v>45595</v>
       </c>
-      <c r="D6">
-        <v>83</v>
-      </c>
-      <c r="E6">
-        <v>149.57317073170731</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="3">
+        <v>92296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>33338</v>
@@ -562,16 +548,13 @@
       <c r="C7" s="2">
         <v>45593</v>
       </c>
-      <c r="D7">
-        <v>84</v>
-      </c>
-      <c r="E7">
-        <v>147.65060240963859</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="3">
+        <v>93408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>34625</v>
@@ -579,16 +562,13 @@
       <c r="C8" s="2">
         <v>45593</v>
       </c>
-      <c r="D8">
-        <v>83</v>
-      </c>
-      <c r="E8">
-        <v>133.7560975609756</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="3">
+        <v>92296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>33338</v>
@@ -596,16 +576,13 @@
       <c r="C9" s="2">
         <v>45594</v>
       </c>
-      <c r="D9">
-        <v>82</v>
-      </c>
-      <c r="E9">
-        <v>151.3086419753086</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="3">
+        <v>91184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>33338</v>
@@ -613,16 +590,13 @@
       <c r="C10" s="2">
         <v>45594</v>
       </c>
-      <c r="D10">
-        <v>83</v>
-      </c>
-      <c r="E10">
-        <v>149.46341463414629</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="3">
+        <v>92296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>33337</v>
@@ -630,11 +604,8 @@
       <c r="C11" s="2">
         <v>45593</v>
       </c>
-      <c r="D11">
-        <v>83</v>
-      </c>
-      <c r="E11">
-        <v>149.46341463414629</v>
+      <c r="D11" s="3">
+        <v>92296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>